<commit_message>
Aggiornamento del file report-checklist.xlsx
Aggiornata row per test case #45

Come richiesto tramite mail del
18 nov 2025, 16:37
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan/Projects/it-fse-accreditamento/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49CAF83-933B-EA44-AE8A-A9569B75615A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F81B84-4C08-9542-8CE6-33426D320E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="35060" windowHeight="19320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35060" windowHeight="19320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="216">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -793,9 +793,6 @@
       <t xml:space="preserve">
 Il software mostra a schermo un messaggio di avviso all'utente finale, invitandolo a riprovare successivamente. L'operatività del software non viene bloccata - la LDO viene comunque generata e resa disponibile nel gestionale.</t>
     </r>
-  </si>
-  <si>
-    <t>Come descritto nella colonna "DESCRIZIONE CASO TEST"</t>
   </si>
   <si>
     <t>2025-11-06T18:50:27+01:00</t>
@@ -2085,7 +2082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2174,6 +2171,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2213,43 +2241,32 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2556,69 +2573,68 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="130.1640625" style="46" customWidth="1"/>
-    <col min="2" max="26" width="8.83203125" style="46" customWidth="1"/>
-    <col min="27" max="16384" width="14.5" style="46"/>
+    <col min="1" max="1" width="130.1640625" customWidth="1"/>
+    <col min="2" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="304" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="33" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="33" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="32" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -2653,51 +2669,51 @@
     <row r="3" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" s="51" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49">
+    <row r="4" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34">
         <v>1</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="51" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52">
+    <row r="5" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
         <v>2</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="51" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52">
+    <row r="6" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36">
         <v>3</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="51" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52">
+    <row r="7" spans="1:2" s="18" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36">
         <v>4</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="51" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52">
+    <row r="8" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="36">
         <v>5</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="37" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="51" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54">
+    <row r="9" spans="1:2" s="18" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="38">
         <v>6</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="39" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3698,11 +3714,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W585"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3752,14 +3768,14 @@
       <c r="W1" s="4"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="48"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
@@ -3780,14 +3796,14 @@
       <c r="W2" s="4"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="48"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -3808,12 +3824,12 @@
       <c r="W3" s="4"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="19"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -3835,12 +3851,12 @@
       <c r="W4" s="4"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="35"/>
+      <c r="D5" s="46"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
@@ -3861,8 +3877,8 @@
       <c r="W5" s="4"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="4"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -4119,62 +4135,58 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="179" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+    <row r="12" spans="1:23" s="64" customFormat="1" ht="179" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="56">
         <v>45</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="24" t="s">
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="N12" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="61" t="s">
+        <v>209</v>
+      </c>
+      <c r="P12" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q12" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="R12" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="O12" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="P12" s="24" t="s">
+      <c r="S12" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="T12" s="56"/>
+      <c r="U12" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="Q12" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="R12" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="S12" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="T12" s="24"/>
-      <c r="U12" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="V12" s="30"/>
-      <c r="W12" s="24" t="s">
+      <c r="V12" s="63"/>
+      <c r="W12" s="56" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4195,16 +4207,16 @@
         <v>87</v>
       </c>
       <c r="F13" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" s="27" t="s">
+      <c r="I13" s="28" t="s">
         <v>143</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>144</v>
       </c>
       <c r="J13" s="24" t="s">
         <v>49</v>
@@ -4218,7 +4230,7 @@
         <v>49</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P13" s="24" t="s">
         <v>49</v>
@@ -4230,7 +4242,7 @@
         <v>49</v>
       </c>
       <c r="S13" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T13" s="24"/>
       <c r="U13" s="29"/>
@@ -4256,16 +4268,16 @@
         <v>88</v>
       </c>
       <c r="F14" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="H14" s="27" t="s">
+      <c r="I14" s="28" t="s">
         <v>148</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>149</v>
       </c>
       <c r="J14" s="24" t="s">
         <v>49</v>
@@ -4279,7 +4291,7 @@
         <v>49</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P14" s="24" t="s">
         <v>49</v>
@@ -4291,7 +4303,7 @@
         <v>49</v>
       </c>
       <c r="S14" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T14" s="24"/>
       <c r="U14" s="29"/>
@@ -4317,16 +4329,16 @@
         <v>89</v>
       </c>
       <c r="F15" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="H15" s="27" t="s">
+      <c r="I15" s="28" t="s">
         <v>153</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>154</v>
       </c>
       <c r="J15" s="24" t="s">
         <v>49</v>
@@ -4340,7 +4352,7 @@
         <v>49</v>
       </c>
       <c r="O15" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P15" s="24" t="s">
         <v>49</v>
@@ -4352,7 +4364,7 @@
         <v>49</v>
       </c>
       <c r="S15" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T15" s="24"/>
       <c r="U15" s="29"/>
@@ -4378,16 +4390,16 @@
         <v>90</v>
       </c>
       <c r="F16" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="H16" s="27" t="s">
+      <c r="I16" s="28" t="s">
         <v>158</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>159</v>
       </c>
       <c r="J16" s="24" t="s">
         <v>49</v>
@@ -4401,7 +4413,7 @@
         <v>49</v>
       </c>
       <c r="O16" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P16" s="24" t="s">
         <v>49</v>
@@ -4413,7 +4425,7 @@
         <v>49</v>
       </c>
       <c r="S16" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T16" s="24"/>
       <c r="U16" s="29"/>
@@ -4439,16 +4451,16 @@
         <v>91</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G17" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="I17" s="28" t="s">
         <v>162</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>163</v>
       </c>
       <c r="J17" s="24" t="s">
         <v>49</v>
@@ -4462,7 +4474,7 @@
         <v>49</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P17" s="24" t="s">
         <v>49</v>
@@ -4474,7 +4486,7 @@
         <v>49</v>
       </c>
       <c r="S17" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T17" s="24"/>
       <c r="U17" s="29"/>
@@ -4500,16 +4512,16 @@
         <v>92</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G18" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H18" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="I18" s="28" t="s">
         <v>168</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>169</v>
       </c>
       <c r="J18" s="24" t="s">
         <v>49</v>
@@ -4523,7 +4535,7 @@
         <v>49</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P18" s="24" t="s">
         <v>49</v>
@@ -4535,7 +4547,7 @@
         <v>49</v>
       </c>
       <c r="S18" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T18" s="24"/>
       <c r="U18" s="29"/>
@@ -4561,16 +4573,16 @@
         <v>93</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G19" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="I19" s="28" t="s">
         <v>174</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>175</v>
       </c>
       <c r="J19" s="24" t="s">
         <v>49</v>
@@ -4584,7 +4596,7 @@
         <v>49</v>
       </c>
       <c r="O19" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P19" s="24" t="s">
         <v>49</v>
@@ -4596,7 +4608,7 @@
         <v>49</v>
       </c>
       <c r="S19" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T19" s="24"/>
       <c r="U19" s="29"/>
@@ -4622,16 +4634,16 @@
         <v>94</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G20" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="H20" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="I20" s="28" t="s">
         <v>179</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>180</v>
       </c>
       <c r="J20" s="24" t="s">
         <v>49</v>
@@ -4645,7 +4657,7 @@
         <v>49</v>
       </c>
       <c r="O20" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P20" s="24" t="s">
         <v>49</v>
@@ -4657,7 +4669,7 @@
         <v>49</v>
       </c>
       <c r="S20" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T20" s="24"/>
       <c r="U20" s="29"/>
@@ -4683,16 +4695,16 @@
         <v>95</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G21" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="H21" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="I21" s="28" t="s">
         <v>185</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>186</v>
       </c>
       <c r="J21" s="24" t="s">
         <v>49</v>
@@ -4706,7 +4718,7 @@
         <v>49</v>
       </c>
       <c r="O21" s="24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P21" s="24" t="s">
         <v>49</v>
@@ -4718,7 +4730,7 @@
         <v>49</v>
       </c>
       <c r="S21" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T21" s="24"/>
       <c r="U21" s="29"/>
@@ -4744,16 +4756,16 @@
         <v>96</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G22" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="H22" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="I22" s="28" t="s">
         <v>191</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>192</v>
       </c>
       <c r="J22" s="24" t="s">
         <v>49</v>
@@ -4767,7 +4779,7 @@
         <v>49</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P22" s="24" t="s">
         <v>49</v>
@@ -4779,7 +4791,7 @@
         <v>49</v>
       </c>
       <c r="S22" s="26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T22" s="24"/>
       <c r="U22" s="29"/>
@@ -4805,16 +4817,16 @@
         <v>104</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G23" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="I23" s="28" t="s">
         <v>203</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>204</v>
       </c>
       <c r="J23" s="24" t="s">
         <v>49</v>
@@ -4852,16 +4864,16 @@
         <v>105</v>
       </c>
       <c r="F24" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="H24" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="G24" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="H24" s="27" t="s">
+      <c r="I24" s="28" t="s">
         <v>208</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>209</v>
       </c>
       <c r="J24" s="24" t="s">
         <v>49</v>
@@ -4899,16 +4911,16 @@
         <v>109</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G25" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="H25" s="24" t="s">
+      <c r="I25" s="24" t="s">
         <v>197</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>198</v>
       </c>
       <c r="J25" s="24" t="s">
         <v>49</v>
@@ -4922,7 +4934,7 @@
         <v>49</v>
       </c>
       <c r="O25" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P25" s="24" t="s">
         <v>49</v>
@@ -4934,7 +4946,7 @@
         <v>49</v>
       </c>
       <c r="S25" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T25" s="24"/>
       <c r="U25" s="24"/>
@@ -9096,143 +9108,143 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="42" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="42" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="42" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="42" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="56" t="s">
+    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="42" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="56" t="s">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="42" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="46" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="56" t="s">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="42" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="46" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="56" t="s">
+    <row r="10" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="42" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="46" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="56" t="s">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="42" t="s">
         <v>115</v>
       </c>
     </row>
@@ -11244,6 +11256,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -11501,28 +11534,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11541,31 +11578,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Aggiunti i test case 191 e 376 non applicabili.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan/Desktop/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/gsd/Progetti/FSE/REPOSITORY it-fse-accreditamento/LDO_LAB/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F0AA9D-843D-6745-B54C-4934C5BD7199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313AEDEB-993F-F24C-A159-1BA0ACB3C9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$42</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="319">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2514,6 +2514,25 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.160125.4.6.6553b9f6de155b156ea1b84785059058609b36fedd25b1e5499385558a7983f1.e075891a55^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST- OK" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST OK - HLA" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>LAB-TRASF non implementato.</t>
   </si>
 </sst>
 </file>
@@ -3002,7 +3021,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3145,6 +3164,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3172,18 +3200,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4629,7 +4645,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W600"/>
+  <dimension ref="A1:W602"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
@@ -4677,14 +4693,14 @@
       <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="55"/>
+      <c r="D2" s="58"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -4705,14 +4721,14 @@
       <c r="W2" s="8"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="62" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="55"/>
+      <c r="D3" s="58"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -4733,12 +4749,12 @@
       <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="62" t="s">
+      <c r="A4" s="61"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="63"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -4760,12 +4776,12 @@
       <c r="W4" s="8"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="62" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="63"/>
+      <c r="D5" s="66"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -4786,8 +4802,8 @@
       <c r="W5" s="8"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="9"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -6421,127 +6437,119 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="42" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34">
-        <v>450</v>
-      </c>
-      <c r="B35" s="34" t="s">
+    <row r="35" spans="1:23" ht="154" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="45">
+        <v>191</v>
+      </c>
+      <c r="B35" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>123</v>
+      <c r="C35" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>314</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F35" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="G35" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="H35" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="I35" s="38" t="s">
-        <v>221</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="38"/>
       <c r="J35" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="L35" s="34" t="s">
+        <v>318</v>
+      </c>
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
       <c r="O35" s="39"/>
       <c r="P35" s="34"/>
       <c r="Q35" s="34"/>
       <c r="R35" s="34"/>
-      <c r="S35" s="36"/>
+      <c r="S35" s="34"/>
       <c r="T35" s="34"/>
       <c r="U35" s="40"/>
-      <c r="V35" s="41"/>
+      <c r="V35" s="47"/>
       <c r="W35" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="42" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34">
-        <v>451</v>
-      </c>
-      <c r="B36" s="34" t="s">
+    <row r="36" spans="1:23" ht="154" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="45">
+        <v>376</v>
+      </c>
+      <c r="B36" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>124</v>
+      <c r="C36" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>316</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="G36" s="37" t="s">
-        <v>222</v>
-      </c>
-      <c r="H36" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="I36" s="38" t="s">
-        <v>225</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="38"/>
       <c r="J36" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
+        <v>86</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="L36" s="34" t="s">
+        <v>318</v>
+      </c>
       <c r="M36" s="34"/>
       <c r="N36" s="34"/>
       <c r="O36" s="39"/>
       <c r="P36" s="34"/>
       <c r="Q36" s="34"/>
       <c r="R36" s="34"/>
-      <c r="S36" s="36"/>
+      <c r="S36" s="34"/>
       <c r="T36" s="34"/>
       <c r="U36" s="40"/>
-      <c r="V36" s="41"/>
+      <c r="V36" s="47"/>
       <c r="W36" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="45">
-        <v>452</v>
-      </c>
-      <c r="B37" s="45" t="s">
+    <row r="37" spans="1:23" s="42" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="34">
+        <v>450</v>
+      </c>
+      <c r="B37" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="45" t="s">
-        <v>119</v>
+      <c r="C37" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="E37" s="36" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="H37" s="37" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>52</v>
@@ -6554,139 +6562,111 @@
       <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="34"/>
-      <c r="S37" s="34"/>
+      <c r="S37" s="36"/>
       <c r="T37" s="34"/>
       <c r="U37" s="40"/>
-      <c r="V37" s="47"/>
+      <c r="V37" s="41"/>
       <c r="W37" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="45">
-        <v>466</v>
-      </c>
-      <c r="B38" s="45" t="s">
+    <row r="38" spans="1:23" s="42" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="34">
+        <v>451</v>
+      </c>
+      <c r="B38" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="E38" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="F38" s="45" t="s">
-        <v>307</v>
-      </c>
-      <c r="G38" s="45" t="s">
-        <v>306</v>
-      </c>
-      <c r="H38" s="45" t="s">
-        <v>308</v>
-      </c>
-      <c r="I38" s="34" t="s">
-        <v>309</v>
+      <c r="C38" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="H38" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="I38" s="38" t="s">
+        <v>225</v>
       </c>
       <c r="J38" s="34" t="s">
         <v>52</v>
       </c>
       <c r="K38" s="34"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="N38" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="O38" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="P38" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q38" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="R38" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="S38" s="36" t="s">
-        <v>275</v>
-      </c>
+      <c r="L38" s="34"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="34"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="34"/>
+      <c r="S38" s="36"/>
       <c r="T38" s="34"/>
-      <c r="U38" s="45"/>
-      <c r="V38" s="45"/>
-      <c r="W38" s="45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" s="42" customFormat="1" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34">
-        <v>467</v>
-      </c>
-      <c r="B39" s="34" t="s">
+      <c r="U38" s="40"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="45">
+        <v>452</v>
+      </c>
+      <c r="B39" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>129</v>
+      <c r="C39" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>119</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="H39" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="I39" s="34" t="s">
-        <v>229</v>
+        <v>120</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="H39" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="I39" s="38" t="s">
+        <v>250</v>
       </c>
       <c r="J39" s="34" t="s">
         <v>52</v>
       </c>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
-      <c r="M39" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="N39" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="O39" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="P39" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q39" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="R39" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="S39" s="36" t="s">
-        <v>242</v>
-      </c>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
       <c r="T39" s="34"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="47"/>
       <c r="W39" s="34" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B40" s="45" t="s">
         <v>34</v>
@@ -6694,29 +6674,29 @@
       <c r="C40" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="48" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>311</v>
-      </c>
-      <c r="G40" s="37" t="s">
-        <v>310</v>
-      </c>
-      <c r="H40" s="37" t="s">
-        <v>312</v>
-      </c>
-      <c r="I40" s="38" t="s">
-        <v>313</v>
+      <c r="D40" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>307</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="H40" s="45" t="s">
+        <v>308</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>309</v>
       </c>
       <c r="J40" s="34" t="s">
         <v>52</v>
       </c>
       <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
+      <c r="L40" s="45"/>
       <c r="M40" s="34" t="s">
         <v>86</v>
       </c>
@@ -6724,7 +6704,7 @@
         <v>52</v>
       </c>
       <c r="O40" s="39" t="s">
-        <v>277</v>
+        <v>171</v>
       </c>
       <c r="P40" s="34" t="s">
         <v>52</v>
@@ -6736,54 +6716,136 @@
         <v>52</v>
       </c>
       <c r="S40" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="T40" s="34"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" s="42" customFormat="1" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34">
+        <v>467</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="H41" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="I41" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="J41" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="N41" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="O41" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="P41" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q41" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="R41" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="S41" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="T41" s="34"/>
+      <c r="U41" s="34"/>
+      <c r="V41" s="34"/>
+      <c r="W41" s="34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="45">
+        <v>473</v>
+      </c>
+      <c r="B42" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="I42" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="N42" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="O42" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="P42" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q42" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="R42" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="S42" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="T40" s="34"/>
-      <c r="U40" s="40"/>
-      <c r="V40" s="47"/>
-      <c r="W40" s="34" t="s">
+      <c r="T42" s="34"/>
+      <c r="U42" s="40"/>
+      <c r="V42" s="47"/>
+      <c r="W42" s="34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="6"/>
-      <c r="U41" s="7"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="8"/>
-    </row>
-    <row r="42" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
-      <c r="T42" s="6"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="8"/>
     </row>
     <row r="43" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="5"/>
@@ -9506,10 +9568,44 @@
       <c r="W178" s="8"/>
     </row>
     <row r="179" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="W179" s="6"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="5"/>
+      <c r="H179" s="5"/>
+      <c r="I179" s="5"/>
+      <c r="J179" s="6"/>
+      <c r="K179" s="6"/>
+      <c r="L179" s="6"/>
+      <c r="M179" s="6"/>
+      <c r="N179" s="6"/>
+      <c r="O179" s="6"/>
+      <c r="P179" s="6"/>
+      <c r="Q179" s="6"/>
+      <c r="R179" s="6"/>
+      <c r="S179" s="6"/>
+      <c r="T179" s="6"/>
+      <c r="U179" s="7"/>
+      <c r="V179" s="2"/>
+      <c r="W179" s="8"/>
     </row>
     <row r="180" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="W180" s="6"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="5"/>
+      <c r="I180" s="5"/>
+      <c r="J180" s="6"/>
+      <c r="K180" s="6"/>
+      <c r="L180" s="6"/>
+      <c r="M180" s="6"/>
+      <c r="N180" s="6"/>
+      <c r="O180" s="6"/>
+      <c r="P180" s="6"/>
+      <c r="Q180" s="6"/>
+      <c r="R180" s="6"/>
+      <c r="S180" s="6"/>
+      <c r="T180" s="6"/>
+      <c r="U180" s="7"/>
+      <c r="V180" s="2"/>
+      <c r="W180" s="8"/>
     </row>
     <row r="181" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="W181" s="6"/>
@@ -10756,13 +10852,19 @@
     <row r="595" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="W595" s="6"/>
     </row>
-    <row r="596" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W596" s="6"/>
+    </row>
+    <row r="597" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W597" s="6"/>
+    </row>
     <row r="598" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="599" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="600" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A9:W40" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W42" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -10783,19 +10885,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J40 P37:R38 P10:R11 J10:J11 M10:N11 M13:N13 P13:R13 J13 J15 M15:N15 P15:R15 M40:N40 J17:J24 M17:N24 P17:R24 J37:J38 M37:N38 P40:R40</xm:sqref>
+          <xm:sqref>J42 P39:R40 P10:R11 J10:J11 M10:N11 M13:N13 P13:R13 J13 J15 M15:N15 P15:R15 M42:N42 J17:J24 M17:N24 P17:R24 J39:J40 M39:N40 P42:R42 J35:J36 P35:R36 M35:N36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T10:T11 T13 T15 T17:T24 T37:T38 T40</xm:sqref>
+          <xm:sqref>T10:T11 T13 T15 T17:T24 T39:T40 T42 T35:T36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DE61C5E-9DA3-4CE3-A1FF-8FBE651EA6B5}">
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K11 K13 K15 K17:K24 K37:K38 K40</xm:sqref>
+          <xm:sqref>K10:K11 K13 K15 K17:K24 K39:K40 K42 K35:K36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10899,31 +11001,31 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="52" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="64" t="s">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="52" t="s">
         <v>132</v>
       </c>
     </row>
@@ -13047,6 +13149,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13304,28 +13427,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13344,31 +13471,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Aggiornati data.json e report-checklist per test case #452
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/gsd/Progetti/FSE/REPOSITORY it-fse-accreditamento/LDO_LAB/A1#111#GESTIONESALUTESRLXX/GESTIONE_SALUTE_SRL/GSD_FSE_Link/1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313AEDEB-993F-F24C-A159-1BA0ACB3C9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8CF14C-29BF-434B-8722-D45361538095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="38400" windowHeight="19300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1705,18 +1705,6 @@
     <t>2.16.840.1.113883.2.9.2.160125.4.6.0dfac52f703e695c2008a99a86c8b1c6cb649e339f51d87022d38d8a139b2588.df98babe91^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-11-26T11:08:54+01:00</t>
-  </si>
-  <si>
-    <t>26/11/2025, 11:08:54</t>
-  </si>
-  <si>
-    <t>56b2b3aa9436f75a041063753b55f4e6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160125.4.6.6553b9f6de155b156ea1b84785059058609b36fedd25b1e5499385558a7983f1.f3d7d4b47f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2025-11-26T11:08:40+01:00</t>
   </si>
   <si>
@@ -2533,6 +2521,18 @@
   </si>
   <si>
     <t>LAB-TRASF non implementato.</t>
+  </si>
+  <si>
+    <t>2025-12-04T18:24:38+01:00</t>
+  </si>
+  <si>
+    <t>04/12/2025, 18:24:38</t>
+  </si>
+  <si>
+    <t>f04a4b3b9bffc354b37320d6a969e2aa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160125.4.6.6553b9f6de155b156ea1b84785059058609b36fedd25b1e5499385558a7983f1.6682012199^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3021,7 +3021,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3201,6 +3201,34 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{565105C8-FFD6-432C-8B2E-BD1D172FCD26}"/>
@@ -4648,10 +4676,10 @@
   <dimension ref="A1:W602"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5002,13 +5030,13 @@
         <v>43</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I11" s="38" t="s">
         <v>157</v>
@@ -5037,7 +5065,7 @@
         <v>52</v>
       </c>
       <c r="S11" s="36" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="T11" s="34"/>
       <c r="U11" s="40"/>
@@ -5124,13 +5152,13 @@
         <v>49</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H13" s="37" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>157</v>
@@ -5159,7 +5187,7 @@
         <v>52</v>
       </c>
       <c r="S13" s="36" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="T13" s="34"/>
       <c r="U13" s="40"/>
@@ -5356,16 +5384,16 @@
         <v>140</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="I17" s="38" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>52</v>
@@ -5391,7 +5419,7 @@
         <v>52</v>
       </c>
       <c r="S17" s="36" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="T17" s="34"/>
       <c r="U17" s="40"/>
@@ -5417,16 +5445,16 @@
         <v>55</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="J18" s="34" t="s">
         <v>52</v>
@@ -5452,7 +5480,7 @@
         <v>52</v>
       </c>
       <c r="S18" s="36" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="T18" s="34"/>
       <c r="U18" s="40"/>
@@ -5478,16 +5506,16 @@
         <v>57</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>52</v>
@@ -5513,7 +5541,7 @@
         <v>52</v>
       </c>
       <c r="S19" s="36" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="T19" s="34"/>
       <c r="U19" s="40"/>
@@ -5539,16 +5567,16 @@
         <v>59</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="J20" s="34" t="s">
         <v>52</v>
@@ -5574,7 +5602,7 @@
         <v>52</v>
       </c>
       <c r="S20" s="36" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="T20" s="34"/>
       <c r="U20" s="40"/>
@@ -5600,16 +5628,16 @@
         <v>61</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J21" s="34" t="s">
         <v>52</v>
@@ -5623,7 +5651,7 @@
         <v>52</v>
       </c>
       <c r="O21" s="39" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="P21" s="34" t="s">
         <v>52</v>
@@ -5635,7 +5663,7 @@
         <v>52</v>
       </c>
       <c r="S21" s="36" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T21" s="34"/>
       <c r="U21" s="40"/>
@@ -5661,16 +5689,16 @@
         <v>63</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J22" s="34" t="s">
         <v>52</v>
@@ -5684,7 +5712,7 @@
         <v>52</v>
       </c>
       <c r="O22" s="39" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="P22" s="34" t="s">
         <v>52</v>
@@ -5696,7 +5724,7 @@
         <v>52</v>
       </c>
       <c r="S22" s="36" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T22" s="34"/>
       <c r="U22" s="40"/>
@@ -5722,16 +5750,16 @@
         <v>65</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J23" s="34" t="s">
         <v>52</v>
@@ -5745,7 +5773,7 @@
         <v>52</v>
       </c>
       <c r="O23" s="39" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="P23" s="34" t="s">
         <v>52</v>
@@ -5757,7 +5785,7 @@
         <v>52</v>
       </c>
       <c r="S23" s="36" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="T23" s="34"/>
       <c r="U23" s="40"/>
@@ -5783,16 +5811,16 @@
         <v>67</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I24" s="38" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="J24" s="34" t="s">
         <v>52</v>
@@ -5806,7 +5834,7 @@
         <v>52</v>
       </c>
       <c r="O24" s="39" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="P24" s="34" t="s">
         <v>52</v>
@@ -5818,7 +5846,7 @@
         <v>52</v>
       </c>
       <c r="S24" s="36" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="T24" s="34"/>
       <c r="U24" s="40"/>
@@ -6448,10 +6476,10 @@
         <v>35</v>
       </c>
       <c r="D35" s="45" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E35" s="36" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
@@ -6464,7 +6492,7 @@
         <v>95</v>
       </c>
       <c r="L35" s="34" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
@@ -6491,10 +6519,10 @@
         <v>35</v>
       </c>
       <c r="D36" s="45" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E36" s="36" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
@@ -6507,7 +6535,7 @@
         <v>95</v>
       </c>
       <c r="L36" s="34" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="M36" s="34"/>
       <c r="N36" s="34"/>
@@ -6617,50 +6645,50 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45">
+    <row r="39" spans="1:23" s="76" customFormat="1" ht="350" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="67">
         <v>452</v>
       </c>
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="48" t="s">
+      <c r="C39" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D39" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="F39" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="G39" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="H39" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="I39" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="J39" s="34" t="s">
+      <c r="F39" s="70" t="s">
+        <v>316</v>
+      </c>
+      <c r="G39" s="70" t="s">
+        <v>315</v>
+      </c>
+      <c r="H39" s="70" t="s">
+        <v>317</v>
+      </c>
+      <c r="I39" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="J39" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="39"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
-      <c r="U39" s="40"/>
-      <c r="V39" s="47"/>
-      <c r="W39" s="34" t="s">
+      <c r="K39" s="72"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="72"/>
+      <c r="Q39" s="72"/>
+      <c r="R39" s="72"/>
+      <c r="S39" s="72"/>
+      <c r="T39" s="72"/>
+      <c r="U39" s="74"/>
+      <c r="V39" s="75"/>
+      <c r="W39" s="72" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6681,16 +6709,16 @@
         <v>138</v>
       </c>
       <c r="F40" s="45" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G40" s="45" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="H40" s="45" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I40" s="34" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J40" s="34" t="s">
         <v>52</v>
@@ -6716,7 +6744,7 @@
         <v>52</v>
       </c>
       <c r="S40" s="36" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="T40" s="34"/>
       <c r="U40" s="45"/>
@@ -6803,16 +6831,16 @@
         <v>144</v>
       </c>
       <c r="F42" s="37" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="I42" s="38" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="J42" s="34" t="s">
         <v>52</v>
@@ -6826,7 +6854,7 @@
         <v>52</v>
       </c>
       <c r="O42" s="39" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="P42" s="34" t="s">
         <v>52</v>
@@ -6838,7 +6866,7 @@
         <v>52</v>
       </c>
       <c r="S42" s="36" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="T42" s="34"/>
       <c r="U42" s="40"/>
@@ -13149,27 +13177,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -13427,10 +13434,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13453,20 +13492,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>